<commit_message>
Updated with Yeti 0.5 RC data.
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="17235" windowHeight="6210"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="17235" windowHeight="6210" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Watchmen" sheetId="1" r:id="rId1"/>
@@ -460,8 +460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,7 +715,7 @@
         <v>1427</v>
       </c>
       <c r="C22">
-        <v>39.299999999999997</v>
+        <v>37.6</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1024,7 +1024,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1276,7 +1276,7 @@
         <v>329</v>
       </c>
       <c r="C22">
-        <v>88.6</v>
+        <v>90.8</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1303,8 +1303,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1557,7 +1557,7 @@
         <v>67</v>
       </c>
       <c r="C22">
-        <v>418.8</v>
+        <v>413.1</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>